<commit_message>
moneda de oro y gato jefe
</commit_message>
<xml_diff>
--- a/diagrama_gantt.xlsx
+++ b/diagrama_gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toni Tormo\Desktop\Uni\4_GTDM\Games\Juego 2D\Games-Juego2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F75EE0-5127-4592-9BDF-8C846BACDC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7B450E-4ECE-4CED-AFDC-571A5535833B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Diseño de Monstruos</t>
   </si>
@@ -98,6 +98,342 @@
   </si>
   <si>
     <t>12 h</t>
+  </si>
+  <si>
+    <r>
+      <t>Planteamiento de Ideas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Esta tarea va al inicio del proyecto.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Creación del GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diseño del Primer Monstruo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, y </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diseño de la Primera Defensa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Estas tareas comienzan después del "Planteamiento de Ideas".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Diseño de Monstruos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diseño de Defensas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Comienzan solo cuando </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diseño del Primer Monstruo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diseño de la Primera Defensa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> han finalizado.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Creación de Mapas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Puede comenzar de forma independiente después de que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diseño de la Primera Defensa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> haya terminado.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Montaje en Unity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Solo se inicia cuando se han completado las tareas de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Creación del GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Creación de Mapas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diseño del Primer Monstruo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diseño de la Primera Defensa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Implementación de Código</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Comienza junto con </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Montaje en Unity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, pero con un día de retraso.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pruebas y Corrección de Errores</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Esta fase se inicia al final, cuando todas las demás tareas están completas.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -156,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -165,6 +501,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,7 +822,7 @@
     <col min="5" max="5" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -501,7 +839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -518,7 +856,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -535,7 +873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -552,7 +890,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -569,7 +907,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -585,8 +923,9 @@
       <c r="E7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -603,7 +942,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -620,7 +959,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -637,7 +976,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -654,7 +993,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -669,6 +1008,41 @@
       </c>
       <c r="E12" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>